<commit_message>
Inicio de mediciones como tal
</commit_message>
<xml_diff>
--- a/Lab/aima-python-master/results_heuristics.xlsx
+++ b/Lab/aima-python-master/results_heuristics.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,47 +462,47 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Time</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Nodes Expanded</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Time per node</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>States Reached</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Nodes in Frontier</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>Solution Cost</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>Solution Length</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" s="2" t="inlineStr">
         <is>
           <t>Reexpanded States</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" s="2" t="inlineStr">
         <is>
           <t>Dummy Nodes</t>
         </is>
@@ -510,30 +510,958 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
+        <v>10.52597212791443</v>
+      </c>
+      <c r="B2" t="n">
+        <v>94232</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.000111702735036022</v>
+      </c>
+      <c r="D2" t="n">
+        <v>257193</v>
+      </c>
+      <c r="E2" t="n">
+        <v>232631</v>
+      </c>
+      <c r="F2" t="n">
+        <v>2085</v>
+      </c>
+      <c r="G2" t="n">
+        <v>17</v>
+      </c>
+      <c r="H2" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2" t="n">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>10.37597727775574</v>
+      </c>
+      <c r="B3" t="n">
+        <v>94232</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.0001101109737430569</v>
+      </c>
+      <c r="D3" t="n">
+        <v>257193</v>
+      </c>
+      <c r="E3" t="n">
+        <v>232631</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2085</v>
+      </c>
+      <c r="G3" t="n">
+        <v>17</v>
+      </c>
+      <c r="H3" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" t="n">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>10.37466263771057</v>
+      </c>
+      <c r="B4" t="n">
+        <v>94232</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.0001100970226431634</v>
+      </c>
+      <c r="D4" t="n">
+        <v>257193</v>
+      </c>
+      <c r="E4" t="n">
+        <v>232631</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2085</v>
+      </c>
+      <c r="G4" t="n">
+        <v>17</v>
+      </c>
+      <c r="H4" t="n">
+        <v>2</v>
+      </c>
+      <c r="I4" t="n">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>10.40870523452759</v>
+      </c>
+      <c r="B5" t="n">
+        <v>94232</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.0001104582862990023</v>
+      </c>
+      <c r="D5" t="n">
+        <v>257193</v>
+      </c>
+      <c r="E5" t="n">
+        <v>232631</v>
+      </c>
+      <c r="F5" t="n">
+        <v>2085</v>
+      </c>
+      <c r="G5" t="n">
+        <v>17</v>
+      </c>
+      <c r="H5" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" t="n">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>10.52128601074219</v>
+      </c>
+      <c r="B6" t="n">
+        <v>94232</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.0001116530054624988</v>
+      </c>
+      <c r="D6" t="n">
+        <v>257193</v>
+      </c>
+      <c r="E6" t="n">
+        <v>232631</v>
+      </c>
+      <c r="F6" t="n">
+        <v>2085</v>
+      </c>
+      <c r="G6" t="n">
+        <v>17</v>
+      </c>
+      <c r="H6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I6" t="n">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>10.17578077316284</v>
+      </c>
+      <c r="B7" t="n">
+        <v>94232</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.0001079864671572591</v>
+      </c>
+      <c r="D7" t="n">
+        <v>257193</v>
+      </c>
+      <c r="E7" t="n">
+        <v>232631</v>
+      </c>
+      <c r="F7" t="n">
+        <v>2085</v>
+      </c>
+      <c r="G7" t="n">
+        <v>17</v>
+      </c>
+      <c r="H7" t="n">
+        <v>2</v>
+      </c>
+      <c r="I7" t="n">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>10.23672270774841</v>
+      </c>
+      <c r="B8" t="n">
+        <v>94232</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.0001086331894446516</v>
+      </c>
+      <c r="D8" t="n">
+        <v>257193</v>
+      </c>
+      <c r="E8" t="n">
+        <v>232631</v>
+      </c>
+      <c r="F8" t="n">
+        <v>2085</v>
+      </c>
+      <c r="G8" t="n">
+        <v>17</v>
+      </c>
+      <c r="H8" t="n">
+        <v>2</v>
+      </c>
+      <c r="I8" t="n">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>10.52879858016968</v>
+      </c>
+      <c r="B9" t="n">
+        <v>94232</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.0001117327296477808</v>
+      </c>
+      <c r="D9" t="n">
+        <v>257193</v>
+      </c>
+      <c r="E9" t="n">
+        <v>232631</v>
+      </c>
+      <c r="F9" t="n">
+        <v>2085</v>
+      </c>
+      <c r="G9" t="n">
+        <v>17</v>
+      </c>
+      <c r="H9" t="n">
+        <v>2</v>
+      </c>
+      <c r="I9" t="n">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>10.26627254486084</v>
+      </c>
+      <c r="B10" t="n">
+        <v>94232</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.0001089467754569662</v>
+      </c>
+      <c r="D10" t="n">
+        <v>257193</v>
+      </c>
+      <c r="E10" t="n">
+        <v>232631</v>
+      </c>
+      <c r="F10" t="n">
+        <v>2085</v>
+      </c>
+      <c r="G10" t="n">
+        <v>17</v>
+      </c>
+      <c r="H10" t="n">
+        <v>2</v>
+      </c>
+      <c r="I10" t="n">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10.30588555335999</v>
+      </c>
+      <c r="B11" t="n">
+        <v>94232</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.0001093671529136597</v>
+      </c>
+      <c r="D11" t="n">
+        <v>257193</v>
+      </c>
+      <c r="E11" t="n">
+        <v>232631</v>
+      </c>
+      <c r="F11" t="n">
+        <v>2085</v>
+      </c>
+      <c r="G11" t="n">
+        <v>17</v>
+      </c>
+      <c r="H11" t="n">
+        <v>2</v>
+      </c>
+      <c r="I11" t="n">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>10.18277382850647</v>
+      </c>
+      <c r="B12" t="n">
+        <v>94232</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.0001080606782038635</v>
+      </c>
+      <c r="D12" t="n">
+        <v>257193</v>
+      </c>
+      <c r="E12" t="n">
+        <v>232631</v>
+      </c>
+      <c r="F12" t="n">
+        <v>2085</v>
+      </c>
+      <c r="G12" t="n">
+        <v>17</v>
+      </c>
+      <c r="H12" t="n">
+        <v>2</v>
+      </c>
+      <c r="I12" t="n">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>10.14780902862549</v>
+      </c>
+      <c r="B13" t="n">
+        <v>94232</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.000107689628031088</v>
+      </c>
+      <c r="D13" t="n">
+        <v>257193</v>
+      </c>
+      <c r="E13" t="n">
+        <v>232631</v>
+      </c>
+      <c r="F13" t="n">
+        <v>2085</v>
+      </c>
+      <c r="G13" t="n">
+        <v>17</v>
+      </c>
+      <c r="H13" t="n">
+        <v>2</v>
+      </c>
+      <c r="I13" t="n">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>10.15396642684937</v>
+      </c>
+      <c r="B14" t="n">
+        <v>94232</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.0001077549709955149</v>
+      </c>
+      <c r="D14" t="n">
+        <v>257193</v>
+      </c>
+      <c r="E14" t="n">
+        <v>232631</v>
+      </c>
+      <c r="F14" t="n">
+        <v>2085</v>
+      </c>
+      <c r="G14" t="n">
+        <v>17</v>
+      </c>
+      <c r="H14" t="n">
+        <v>2</v>
+      </c>
+      <c r="I14" t="n">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>10.43419766426086</v>
+      </c>
+      <c r="B15" t="n">
+        <v>94232</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.0001107288146729441</v>
+      </c>
+      <c r="D15" t="n">
+        <v>257193</v>
+      </c>
+      <c r="E15" t="n">
+        <v>232631</v>
+      </c>
+      <c r="F15" t="n">
+        <v>2085</v>
+      </c>
+      <c r="G15" t="n">
+        <v>17</v>
+      </c>
+      <c r="H15" t="n">
+        <v>2</v>
+      </c>
+      <c r="I15" t="n">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>10.19453835487366</v>
+      </c>
+      <c r="B16" t="n">
+        <v>94232</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.0001081855246081337</v>
+      </c>
+      <c r="D16" t="n">
+        <v>257193</v>
+      </c>
+      <c r="E16" t="n">
+        <v>232631</v>
+      </c>
+      <c r="F16" t="n">
+        <v>2085</v>
+      </c>
+      <c r="G16" t="n">
+        <v>17</v>
+      </c>
+      <c r="H16" t="n">
+        <v>2</v>
+      </c>
+      <c r="I16" t="n">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>10.20782732963562</v>
+      </c>
+      <c r="B17" t="n">
+        <v>94232</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.0001083265486208042</v>
+      </c>
+      <c r="D17" t="n">
+        <v>257193</v>
+      </c>
+      <c r="E17" t="n">
+        <v>232631</v>
+      </c>
+      <c r="F17" t="n">
+        <v>2085</v>
+      </c>
+      <c r="G17" t="n">
+        <v>17</v>
+      </c>
+      <c r="H17" t="n">
+        <v>2</v>
+      </c>
+      <c r="I17" t="n">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>10.0264687538147</v>
+      </c>
+      <c r="B18" t="n">
+        <v>94232</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.0001064019521374342</v>
+      </c>
+      <c r="D18" t="n">
+        <v>257193</v>
+      </c>
+      <c r="E18" t="n">
+        <v>232631</v>
+      </c>
+      <c r="F18" t="n">
+        <v>2085</v>
+      </c>
+      <c r="G18" t="n">
+        <v>17</v>
+      </c>
+      <c r="H18" t="n">
+        <v>2</v>
+      </c>
+      <c r="I18" t="n">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>10.43945503234863</v>
+      </c>
+      <c r="B19" t="n">
+        <v>94232</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.0001107846064219016</v>
+      </c>
+      <c r="D19" t="n">
+        <v>257193</v>
+      </c>
+      <c r="E19" t="n">
+        <v>232631</v>
+      </c>
+      <c r="F19" t="n">
+        <v>2085</v>
+      </c>
+      <c r="G19" t="n">
+        <v>17</v>
+      </c>
+      <c r="H19" t="n">
+        <v>2</v>
+      </c>
+      <c r="I19" t="n">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>10.24201154708862</v>
+      </c>
+      <c r="B20" t="n">
+        <v>94232</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.0001086893151698852</v>
+      </c>
+      <c r="D20" t="n">
+        <v>257193</v>
+      </c>
+      <c r="E20" t="n">
+        <v>232631</v>
+      </c>
+      <c r="F20" t="n">
+        <v>2085</v>
+      </c>
+      <c r="G20" t="n">
+        <v>17</v>
+      </c>
+      <c r="H20" t="n">
+        <v>2</v>
+      </c>
+      <c r="I20" t="n">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>10.33277273178101</v>
+      </c>
+      <c r="B21" t="n">
+        <v>94232</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.0001096524825089248</v>
+      </c>
+      <c r="D21" t="n">
+        <v>257193</v>
+      </c>
+      <c r="E21" t="n">
+        <v>232631</v>
+      </c>
+      <c r="F21" t="n">
+        <v>2085</v>
+      </c>
+      <c r="G21" t="n">
+        <v>17</v>
+      </c>
+      <c r="H21" t="n">
+        <v>2</v>
+      </c>
+      <c r="I21" t="n">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>10.370525598526</v>
+      </c>
+      <c r="B22" t="n">
+        <v>94232</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.0001100531199436073</v>
+      </c>
+      <c r="D22" t="n">
+        <v>257193</v>
+      </c>
+      <c r="E22" t="n">
+        <v>232631</v>
+      </c>
+      <c r="F22" t="n">
+        <v>2085</v>
+      </c>
+      <c r="G22" t="n">
+        <v>17</v>
+      </c>
+      <c r="H22" t="n">
+        <v>2</v>
+      </c>
+      <c r="I22" t="n">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>10.31395268440247</v>
+      </c>
+      <c r="B23" t="n">
+        <v>94232</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.0001094527621657448</v>
+      </c>
+      <c r="D23" t="n">
+        <v>257193</v>
+      </c>
+      <c r="E23" t="n">
+        <v>232631</v>
+      </c>
+      <c r="F23" t="n">
+        <v>2085</v>
+      </c>
+      <c r="G23" t="n">
+        <v>17</v>
+      </c>
+      <c r="H23" t="n">
+        <v>2</v>
+      </c>
+      <c r="I23" t="n">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>10.34682393074036</v>
+      </c>
+      <c r="B24" t="n">
+        <v>94232</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.0001098015953257954</v>
+      </c>
+      <c r="D24" t="n">
+        <v>257193</v>
+      </c>
+      <c r="E24" t="n">
+        <v>232631</v>
+      </c>
+      <c r="F24" t="n">
+        <v>2085</v>
+      </c>
+      <c r="G24" t="n">
+        <v>17</v>
+      </c>
+      <c r="H24" t="n">
+        <v>2</v>
+      </c>
+      <c r="I24" t="n">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>10.90882158279419</v>
+      </c>
+      <c r="B25" t="n">
+        <v>94232</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.0001157655741446026</v>
+      </c>
+      <c r="D25" t="n">
+        <v>257193</v>
+      </c>
+      <c r="E25" t="n">
+        <v>232631</v>
+      </c>
+      <c r="F25" t="n">
+        <v>2085</v>
+      </c>
+      <c r="G25" t="n">
+        <v>17</v>
+      </c>
+      <c r="H25" t="n">
+        <v>2</v>
+      </c>
+      <c r="I25" t="n">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>10.74855732917786</v>
+      </c>
+      <c r="B26" t="n">
+        <v>94232</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.0001140648328506012</v>
+      </c>
+      <c r="D26" t="n">
+        <v>257193</v>
+      </c>
+      <c r="E26" t="n">
+        <v>232631</v>
+      </c>
+      <c r="F26" t="n">
+        <v>2085</v>
+      </c>
+      <c r="G26" t="n">
+        <v>17</v>
+      </c>
+      <c r="H26" t="n">
+        <v>2</v>
+      </c>
+      <c r="I26" t="n">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>10.24333190917969</v>
+      </c>
+      <c r="B27" t="n">
+        <v>94232</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.000108703326992738</v>
+      </c>
+      <c r="D27" t="n">
+        <v>257193</v>
+      </c>
+      <c r="E27" t="n">
+        <v>232631</v>
+      </c>
+      <c r="F27" t="n">
+        <v>2085</v>
+      </c>
+      <c r="G27" t="n">
+        <v>17</v>
+      </c>
+      <c r="H27" t="n">
+        <v>2</v>
+      </c>
+      <c r="I27" t="n">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>10.49409675598145</v>
+      </c>
+      <c r="B28" t="n">
+        <v>94232</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.0001113644702010086</v>
+      </c>
+      <c r="D28" t="n">
+        <v>257193</v>
+      </c>
+      <c r="E28" t="n">
+        <v>232631</v>
+      </c>
+      <c r="F28" t="n">
+        <v>2085</v>
+      </c>
+      <c r="G28" t="n">
+        <v>17</v>
+      </c>
+      <c r="H28" t="n">
+        <v>2</v>
+      </c>
+      <c r="I28" t="n">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>10.39191937446594</v>
+      </c>
+      <c r="B29" t="n">
+        <v>94232</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.0001102801529678447</v>
+      </c>
+      <c r="D29" t="n">
+        <v>257193</v>
+      </c>
+      <c r="E29" t="n">
+        <v>232631</v>
+      </c>
+      <c r="F29" t="n">
+        <v>2085</v>
+      </c>
+      <c r="G29" t="n">
+        <v>17</v>
+      </c>
+      <c r="H29" t="n">
+        <v>2</v>
+      </c>
+      <c r="I29" t="n">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>10.60492515563965</v>
+      </c>
+      <c r="B30" t="n">
+        <v>94232</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.000112540592958227</v>
+      </c>
+      <c r="D30" t="n">
+        <v>257193</v>
+      </c>
+      <c r="E30" t="n">
+        <v>232631</v>
+      </c>
+      <c r="F30" t="n">
+        <v>2085</v>
+      </c>
+      <c r="G30" t="n">
+        <v>17</v>
+      </c>
+      <c r="H30" t="n">
+        <v>2</v>
+      </c>
+      <c r="I30" t="n">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>10.70121288299561</v>
+      </c>
+      <c r="B31" t="n">
+        <v>94232</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.0001135624085554335</v>
+      </c>
+      <c r="D31" t="n">
+        <v>257193</v>
+      </c>
+      <c r="E31" t="n">
+        <v>232631</v>
+      </c>
+      <c r="F31" t="n">
+        <v>2085</v>
+      </c>
+      <c r="G31" t="n">
+        <v>17</v>
+      </c>
+      <c r="H31" t="n">
+        <v>2</v>
+      </c>
+      <c r="I31" t="n">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>10.58208656311035</v>
+      </c>
+      <c r="B32" t="n">
+        <v>94232</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.0001122982273867726</v>
+      </c>
+      <c r="D32" t="n">
+        <v>257193</v>
+      </c>
+      <c r="E32" t="n">
+        <v>232631</v>
+      </c>
+      <c r="F32" t="n">
+        <v>2085</v>
+      </c>
+      <c r="G32" t="n">
+        <v>17</v>
+      </c>
+      <c r="H32" t="n">
+        <v>2</v>
+      </c>
+      <c r="I32" t="n">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>10.62032890319824</v>
+      </c>
+      <c r="B33" t="n">
+        <v>94232</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.0001127040591645963</v>
+      </c>
+      <c r="D33" t="n">
+        <v>257193</v>
+      </c>
+      <c r="E33" t="n">
+        <v>232631</v>
+      </c>
+      <c r="F33" t="n">
+        <v>2085</v>
+      </c>
+      <c r="G33" t="n">
+        <v>17</v>
+      </c>
+      <c r="H33" t="n">
+        <v>2</v>
+      </c>
+      <c r="I33" t="n">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
         <v>20.14047312736511</v>
       </c>
-      <c r="B2" t="n">
-        <v>94232</v>
-      </c>
-      <c r="C2" t="n">
+      <c r="B34" t="n">
+        <v>94232</v>
+      </c>
+      <c r="C34" t="n">
         <v>0.0002137328415757398</v>
       </c>
-      <c r="D2" t="n">
-        <v>257193</v>
-      </c>
-      <c r="E2" t="n">
-        <v>232631</v>
-      </c>
-      <c r="F2" t="n">
-        <v>2085</v>
-      </c>
-      <c r="G2" t="n">
-        <v>17</v>
-      </c>
-      <c r="H2" t="n">
-        <v>2</v>
-      </c>
-      <c r="I2" t="n">
+      <c r="D34" t="n">
+        <v>257193</v>
+      </c>
+      <c r="E34" t="n">
+        <v>232631</v>
+      </c>
+      <c r="F34" t="n">
+        <v>2085</v>
+      </c>
+      <c r="G34" t="n">
+        <v>17</v>
+      </c>
+      <c r="H34" t="n">
+        <v>2</v>
+      </c>
+      <c r="I34" t="n">
         <v>31000</v>
       </c>
     </row>

</xml_diff>